<commit_message>
Se actualiza grafico y tabla de tiempos
La tabla y el grafico se actualiza con los resultados del test nuevo
</commit_message>
<xml_diff>
--- a/ComplejidadComputacional/documentacion/GraficosEnElTrabajo.xlsx
+++ b/ComplejidadComputacional/documentacion/GraficosEnElTrabajo.xlsx
@@ -49,7 +49,7 @@
     <t>EvaluarHorner</t>
   </si>
   <si>
-    <t>A partir de 24000 elementos me dio stackoverflow</t>
+    <t>A partir de 23000 elementos me dio stackoverflow</t>
   </si>
 </sst>
 </file>
@@ -139,35 +139,133 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="70000"/>
+                </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="38000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:tint val="50000"/>
+                      <a:satMod val="300000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="35000">
+                    <a:schemeClr val="accent1">
+                      <a:tint val="37000"/>
+                      <a:satMod val="300000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:tint val="15000"/>
+                      <a:satMod val="350000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="1"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent1">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="38000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$1:$R$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1550.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3050.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4550.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6050.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7550.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9050.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10550.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12050.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13550.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15050.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16550.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18050.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19550.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21050.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22550.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$B$2:$Q$2</c:f>
+              <c:f>Hoja1!$B$2:$R$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -196,25 +294,28 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.0</c:v>
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -236,82 +337,183 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent2">
+                  <a:alpha val="70000"/>
+                </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="38000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:tint val="50000"/>
+                      <a:satMod val="300000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="35000">
+                    <a:schemeClr val="accent2">
+                      <a:tint val="37000"/>
+                      <a:satMod val="300000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:tint val="15000"/>
+                      <a:satMod val="350000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="1"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent2">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="38000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$1:$R$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1550.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3050.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4550.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6050.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7550.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9050.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10550.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12050.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13550.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15050.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16550.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18050.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19550.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21050.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22550.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$B$3:$Q$3</c:f>
+              <c:f>Hoja1!$B$3:$R$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.0</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49.0</c:v>
+                  <c:v>88.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>184.0</c:v>
+                  <c:v>259.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>399.0</c:v>
+                  <c:v>532.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>767.0</c:v>
+                  <c:v>906.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1183.0</c:v>
+                  <c:v>1470.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1830.0</c:v>
+                  <c:v>1953.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3307.0</c:v>
+                  <c:v>2862.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4283.0</c:v>
+                  <c:v>3561.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5283.0</c:v>
+                  <c:v>4459.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6594.0</c:v>
+                  <c:v>5370.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7983.0</c:v>
+                  <c:v>6356.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9287.0</c:v>
+                  <c:v>7742.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9111.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -333,82 +535,183 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent3">
+                  <a:alpha val="70000"/>
+                </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="38000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:tint val="50000"/>
+                      <a:satMod val="300000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="35000">
+                    <a:schemeClr val="accent3">
+                      <a:tint val="37000"/>
+                      <a:satMod val="300000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:tint val="15000"/>
+                      <a:satMod val="350000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="1"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
-                  <a:schemeClr val="accent3"/>
+                  <a:schemeClr val="accent3">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="38000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$1:$R$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1550.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3050.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4550.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6050.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7550.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9050.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10550.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12050.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13550.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15050.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16550.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18050.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19550.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21050.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22550.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$B$4:$Q$4</c:f>
+              <c:f>Hoja1!$B$4:$R$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26.0</c:v>
+                  <c:v>33.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>51.0</c:v>
+                  <c:v>61.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>93.0</c:v>
+                  <c:v>101.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>139.0</c:v>
+                  <c:v>149.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>168.0</c:v>
+                  <c:v>196.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>249.0</c:v>
+                  <c:v>253.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>387.0</c:v>
+                  <c:v>315.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>448.0</c:v>
+                  <c:v>410.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>556.0</c:v>
+                  <c:v>484.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>683.0</c:v>
+                  <c:v>561.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>804.0</c:v>
+                  <c:v>680.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>950.0</c:v>
+                  <c:v>819.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>936.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -430,82 +733,183 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent4">
+                  <a:alpha val="70000"/>
+                </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="38000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="50000"/>
+                      <a:satMod val="300000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="35000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="37000"/>
+                      <a:satMod val="300000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="15000"/>
+                      <a:satMod val="350000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="1"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
-                  <a:schemeClr val="accent4"/>
+                  <a:schemeClr val="accent4">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="38000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$1:$R$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1550.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3050.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4550.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6050.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7550.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9050.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10550.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12050.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13550.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15050.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16550.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18050.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19550.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21050.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22550.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$B$5:$Q$5</c:f>
+              <c:f>Hoja1!$B$5:$R$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>52.0</c:v>
+                  <c:v>88.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>192.0</c:v>
+                  <c:v>269.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>435.0</c:v>
+                  <c:v>552.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>764.0</c:v>
+                  <c:v>898.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1163.0</c:v>
+                  <c:v>1353.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1998.0</c:v>
+                  <c:v>2089.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3397.0</c:v>
+                  <c:v>2710.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4115.0</c:v>
+                  <c:v>3480.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5176.0</c:v>
+                  <c:v>4435.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7049.0</c:v>
+                  <c:v>5209.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8208.0</c:v>
+                  <c:v>6481.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9541.0</c:v>
+                  <c:v>7759.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9443.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -527,82 +931,183 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:schemeClr val="accent5">
+                  <a:alpha val="70000"/>
+                </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="38000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:tint val="50000"/>
+                      <a:satMod val="300000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="35000">
+                    <a:schemeClr val="accent5">
+                      <a:tint val="37000"/>
+                      <a:satMod val="300000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:tint val="15000"/>
+                      <a:satMod val="350000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="1"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
-                  <a:schemeClr val="accent5"/>
+                  <a:schemeClr val="accent5">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="38000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$1:$R$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1550.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3050.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4550.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6050.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7550.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9050.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10550.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12050.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13550.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15050.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16550.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18050.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19550.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21050.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22550.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$B$6:$Q$6</c:f>
+              <c:f>Hoja1!$B$6:$R$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.0</c:v>
+                  <c:v>55.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>130.0</c:v>
+                  <c:v>191.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>324.0</c:v>
+                  <c:v>404.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>622.0</c:v>
+                  <c:v>733.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>962.0</c:v>
+                  <c:v>1069.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1613.0</c:v>
+                  <c:v>1622.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3016.0</c:v>
+                  <c:v>2211.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3560.0</c:v>
+                  <c:v>2895.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4634.0</c:v>
+                  <c:v>3484.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6010.0</c:v>
+                  <c:v>4404.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7020.0</c:v>
+                  <c:v>5142.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8368.0</c:v>
+                  <c:v>6330.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7400.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -624,82 +1129,183 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="accent6">
+                  <a:alpha val="70000"/>
+                </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="38000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:tint val="50000"/>
+                      <a:satMod val="300000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="35000">
+                    <a:schemeClr val="accent6">
+                      <a:tint val="37000"/>
+                      <a:satMod val="300000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:tint val="15000"/>
+                      <a:satMod val="350000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="1"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
-                  <a:schemeClr val="accent6"/>
+                  <a:schemeClr val="accent6">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="38000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$1:$R$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1550.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3050.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4550.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6050.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7550.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9050.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10550.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12050.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13550.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15050.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16550.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18050.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19550.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21050.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22550.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$B$7:$Q$7</c:f>
+              <c:f>Hoja1!$B$7:$R$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26.0</c:v>
+                  <c:v>33.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>47.0</c:v>
+                  <c:v>63.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>78.0</c:v>
+                  <c:v>99.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>121.0</c:v>
+                  <c:v>141.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>172.0</c:v>
+                  <c:v>193.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>242.0</c:v>
+                  <c:v>264.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>387.0</c:v>
+                  <c:v>318.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>482.0</c:v>
+                  <c:v>404.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>566.0</c:v>
+                  <c:v>470.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>664.0</c:v>
+                  <c:v>604.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>803.0</c:v>
+                  <c:v>666.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>896.0</c:v>
+                  <c:v>794.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>973.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -721,41 +1327,138 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent1">
                   <a:lumMod val="60000"/>
+                  <a:alpha val="70000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="38000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                      <a:tint val="50000"/>
+                      <a:satMod val="300000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="35000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                      <a:tint val="37000"/>
+                      <a:satMod val="300000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                      <a:tint val="15000"/>
+                      <a:satMod val="350000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="1"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
                   <a:schemeClr val="accent1">
                     <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="38000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$1:$R$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1550.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3050.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4550.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6050.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7550.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9050.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10550.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12050.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13550.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15050.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16550.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18050.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19550.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21050.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22550.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$B$8:$Q$8</c:f>
+              <c:f>Hoja1!$B$8:$R$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -763,7 +1466,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.0</c:v>
@@ -775,34 +1478,37 @@
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>10.0</c:v>
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -817,11 +1523,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2129205376"/>
-        <c:axId val="-2129196992"/>
+        <c:axId val="-2107969232"/>
+        <c:axId val="-2108068800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2129205376"/>
+        <c:axId val="-2107969232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -831,7 +1537,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -845,7 +1551,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="5000"/>
                   <a:lumOff val="95000"/>
                 </a:schemeClr>
@@ -862,9 +1568,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
+                      <a:schemeClr val="dk1">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
@@ -876,15 +1582,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Cantidad de</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> </a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>elementos</a:t>
+                  <a:t>Cantidad de Elementos</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -903,9 +1601,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
+                    <a:schemeClr val="dk1">
                       <a:lumMod val="65000"/>
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
@@ -925,11 +1623,11 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9525" cap="rnd">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -943,7 +1641,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:schemeClr val="dk1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -956,12 +1654,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2129196992"/>
+        <c:crossAx val="-2108068800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2129196992"/>
+        <c:axId val="-2108068800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -971,7 +1669,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -985,7 +1683,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="5000"/>
                   <a:lumOff val="95000"/>
                 </a:schemeClr>
@@ -1002,9 +1700,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
+                      <a:schemeClr val="dk1">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
@@ -1020,12 +1718,9 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> en </a:t>
+                  <a:t> en Milisegundos</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Milisegundos</a:t>
-                </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1043,9 +1738,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
+                    <a:schemeClr val="dk1">
                       <a:lumMod val="65000"/>
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
@@ -1065,8 +1760,14 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1075,9 +1776,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:schemeClr val="dk1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -1090,12 +1791,26 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2129205376"/>
+        <c:crossAx val="-2107969232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
-        <a:noFill/>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:alpha val="0"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -1118,9 +1833,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
@@ -1140,11 +1855,11 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="lt1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="dk1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -1212,33 +1927,56 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="246">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1247,38 +1985,15 @@
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1312,49 +2027,66 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="1"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="1"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="2"/>
+    <cs:effectRef idx="1"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:alpha val="70000"/>
+          </a:schemeClr>
         </a:solidFill>
+        <a:prstDash val="sysDot"/>
         <a:round/>
       </a:ln>
     </cs:spPr>
@@ -1363,21 +2095,21 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="2">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="1"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
@@ -1386,10 +2118,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1405,16 +2137,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1434,17 +2165,18 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1453,12 +2185,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -1472,12 +2204,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -1491,26 +2223,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1524,12 +2250,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
@@ -1543,14 +2269,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1562,12 +2288,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -1581,27 +2307,44 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" spc="0" baseline="0"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1">
+              <a:alpha val="0"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </cs:spPr>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -1609,11 +2352,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1621,12 +2375,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -1640,12 +2394,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1654,14 +2408,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1670,7 +2423,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -1688,14 +2441,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
   </cs:upBar>
   <cs:valueAxis>
@@ -1703,26 +2448,31 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" spc="0" baseline="0"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1732,19 +2482,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2049,10 +2799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+      <selection activeCell="V23" sqref="V23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2061,57 +2811,63 @@
     <col min="2" max="10" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C1">
-        <v>500</v>
+        <v>1550</v>
       </c>
       <c r="D1">
-        <v>1000</v>
+        <v>3050</v>
       </c>
       <c r="E1">
         <v>2500</v>
       </c>
       <c r="F1">
-        <v>4000</v>
+        <v>4550</v>
       </c>
       <c r="G1">
-        <v>5500</v>
+        <v>6050</v>
       </c>
       <c r="H1">
-        <v>7000</v>
+        <v>7550</v>
       </c>
       <c r="I1">
-        <v>8500</v>
+        <v>9050</v>
       </c>
       <c r="J1">
-        <v>10000</v>
+        <v>10550</v>
       </c>
       <c r="K1">
-        <v>12000</v>
+        <v>12050</v>
       </c>
       <c r="L1">
-        <v>15000</v>
+        <v>13550</v>
       </c>
       <c r="M1">
-        <v>16500</v>
+        <v>15050</v>
       </c>
       <c r="N1">
-        <v>18000</v>
+        <v>16550</v>
       </c>
       <c r="O1">
-        <v>20000</v>
+        <v>18050</v>
       </c>
       <c r="P1">
-        <v>21500</v>
+        <v>19550</v>
       </c>
       <c r="Q1">
-        <v>23000</v>
+        <v>21050</v>
+      </c>
+      <c r="R1">
+        <v>22550</v>
+      </c>
+      <c r="T1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2143,84 +2899,87 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="S2" t="s">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="E3">
         <v>14</v>
       </c>
       <c r="F3">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="G3">
-        <v>184</v>
+        <v>259</v>
       </c>
       <c r="H3">
-        <v>399</v>
+        <v>532</v>
       </c>
       <c r="I3">
-        <v>767</v>
+        <v>906</v>
       </c>
       <c r="J3">
-        <v>1183</v>
+        <v>1470</v>
       </c>
       <c r="K3">
-        <v>1830</v>
+        <v>1953</v>
       </c>
       <c r="L3">
-        <v>3307</v>
+        <v>2862</v>
       </c>
       <c r="M3">
-        <v>4283</v>
+        <v>3561</v>
       </c>
       <c r="N3">
-        <v>5283</v>
+        <v>4459</v>
       </c>
       <c r="O3">
-        <v>6594</v>
+        <v>5370</v>
       </c>
       <c r="P3">
-        <v>7983</v>
+        <v>6356</v>
       </c>
       <c r="Q3">
-        <v>9287</v>
+        <v>7742</v>
+      </c>
+      <c r="R3">
+        <v>9111</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2228,52 +2987,55 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E4">
         <v>11</v>
       </c>
       <c r="F4">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="G4">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="H4">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="I4">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="J4">
-        <v>168</v>
+        <v>196</v>
       </c>
       <c r="K4">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="L4">
-        <v>387</v>
+        <v>315</v>
       </c>
       <c r="M4">
-        <v>448</v>
+        <v>410</v>
       </c>
       <c r="N4">
-        <v>556</v>
+        <v>484</v>
       </c>
       <c r="O4">
-        <v>683</v>
+        <v>561</v>
       </c>
       <c r="P4">
-        <v>804</v>
+        <v>680</v>
       </c>
       <c r="Q4">
-        <v>950</v>
+        <v>819</v>
+      </c>
+      <c r="R4">
+        <v>936</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2281,52 +3043,55 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E5">
         <v>16</v>
       </c>
       <c r="F5">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="G5">
-        <v>192</v>
+        <v>269</v>
       </c>
       <c r="H5">
-        <v>435</v>
+        <v>552</v>
       </c>
       <c r="I5">
-        <v>764</v>
+        <v>898</v>
       </c>
       <c r="J5">
-        <v>1163</v>
+        <v>1353</v>
       </c>
       <c r="K5">
-        <v>1998</v>
+        <v>2089</v>
       </c>
       <c r="L5">
-        <v>3397</v>
+        <v>2710</v>
       </c>
       <c r="M5">
-        <v>4115</v>
+        <v>3480</v>
       </c>
       <c r="N5">
-        <v>5176</v>
+        <v>4435</v>
       </c>
       <c r="O5">
-        <v>7049</v>
+        <v>5209</v>
       </c>
       <c r="P5">
-        <v>8208</v>
+        <v>6481</v>
       </c>
       <c r="Q5">
-        <v>9541</v>
+        <v>7759</v>
+      </c>
+      <c r="R5">
+        <v>9443</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -2334,52 +3099,55 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E6">
         <v>6</v>
       </c>
       <c r="F6">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="G6">
-        <v>130</v>
+        <v>191</v>
       </c>
       <c r="H6">
-        <v>324</v>
+        <v>404</v>
       </c>
       <c r="I6">
-        <v>622</v>
+        <v>733</v>
       </c>
       <c r="J6">
-        <v>962</v>
+        <v>1069</v>
       </c>
       <c r="K6">
-        <v>1613</v>
+        <v>1622</v>
       </c>
       <c r="L6">
-        <v>3016</v>
+        <v>2211</v>
       </c>
       <c r="M6">
-        <v>3560</v>
+        <v>2895</v>
       </c>
       <c r="N6">
-        <v>4634</v>
+        <v>3484</v>
       </c>
       <c r="O6">
-        <v>6010</v>
+        <v>4404</v>
       </c>
       <c r="P6">
-        <v>7020</v>
+        <v>5142</v>
       </c>
       <c r="Q6">
-        <v>8368</v>
+        <v>6330</v>
+      </c>
+      <c r="R6">
+        <v>7400</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2387,52 +3155,55 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <v>10</v>
       </c>
       <c r="F7">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="G7">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="H7">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="I7">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="J7">
-        <v>172</v>
+        <v>193</v>
       </c>
       <c r="K7">
-        <v>242</v>
+        <v>264</v>
       </c>
       <c r="L7">
-        <v>387</v>
+        <v>318</v>
       </c>
       <c r="M7">
-        <v>482</v>
+        <v>404</v>
       </c>
       <c r="N7">
-        <v>566</v>
+        <v>470</v>
       </c>
       <c r="O7">
-        <v>664</v>
+        <v>604</v>
       </c>
       <c r="P7">
-        <v>803</v>
+        <v>666</v>
       </c>
       <c r="Q7">
-        <v>896</v>
+        <v>794</v>
+      </c>
+      <c r="R7">
+        <v>973</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -2443,7 +3214,7 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -2455,34 +3226,37 @@
         <v>2</v>
       </c>
       <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="J8">
         <v>3</v>
-      </c>
-      <c r="I8">
-        <v>3</v>
-      </c>
-      <c r="J8">
-        <v>4</v>
       </c>
       <c r="K8">
         <v>4</v>
       </c>
       <c r="L8">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M8">
+        <v>5</v>
+      </c>
+      <c r="N8">
         <v>7</v>
-      </c>
-      <c r="N8">
-        <v>6</v>
       </c>
       <c r="O8">
         <v>8</v>
       </c>
       <c r="P8">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q8">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="R8">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>